<commit_message>
Update test with activity specific code
</commit_message>
<xml_diff>
--- a/tests/dev/01_MeanModel_Raltegravir/workflow-input-01.xlsx
+++ b/tests/dev/01_MeanModel_Raltegravir/workflow-input-01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" tabRatio="863" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" tabRatio="863" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="_readme" sheetId="8" r:id="rId1"/>
@@ -418,7 +418,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="319">
   <si>
     <t>reportName</t>
   </si>
@@ -1738,12 +1738,47 @@
   <si>
     <t>PKML/Raltegravir 50 mg  (lactose formulation).pkml</t>
   </si>
+  <si>
+    <t>Activity specific code</t>
+  </si>
+  <si>
+    <t>activitySpecificCode</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Leave empty if there is no activity specific code.
+Otherwise: the name of the R function which will be called directly before </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>workflow$runWorkflow()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> in the generated R code.
+This function must be placed in the same directory as the generated R code and must have 1 argument of the type "workflow".
+It can modify the created workflow directly before execution (e.g. change options, add user-defined tasks, ...)</t>
+    </r>
+  </si>
+  <si>
+    <t>myUserFunction</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1819,6 +1854,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1879,7 +1920,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1952,6 +1993,13 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3376,7 +3424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -3417,11 +3465,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3696,7 +3744,28 @@
         <v>150</v>
       </c>
     </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="36" t="s">
+        <v>315</v>
+      </c>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+    </row>
+    <row r="30" spans="1:3" ht="51.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="37" t="s">
+        <v>316</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>317</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>318</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A29:C29"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>

</xml_diff>

<commit_message>
369 activity specific code (#388)
* Fixes #369 accounts for activitySpecificCode in Excel template

* Update test with activity specific code
</commit_message>
<xml_diff>
--- a/tests/dev/01_MeanModel_Raltegravir/workflow-input-01.xlsx
+++ b/tests/dev/01_MeanModel_Raltegravir/workflow-input-01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" tabRatio="863" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" tabRatio="863" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="_readme" sheetId="8" r:id="rId1"/>
@@ -418,7 +418,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="319">
   <si>
     <t>reportName</t>
   </si>
@@ -1738,12 +1738,47 @@
   <si>
     <t>PKML/Raltegravir 50 mg  (lactose formulation).pkml</t>
   </si>
+  <si>
+    <t>Activity specific code</t>
+  </si>
+  <si>
+    <t>activitySpecificCode</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Leave empty if there is no activity specific code.
+Otherwise: the name of the R function which will be called directly before </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t>workflow$runWorkflow()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> in the generated R code.
+This function must be placed in the same directory as the generated R code and must have 1 argument of the type "workflow".
+It can modify the created workflow directly before execution (e.g. change options, add user-defined tasks, ...)</t>
+    </r>
+  </si>
+  <si>
+    <t>myUserFunction</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1819,6 +1854,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1879,7 +1920,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1952,6 +1993,13 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3376,7 +3424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -3417,11 +3465,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3696,7 +3744,28 @@
         <v>150</v>
       </c>
     </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="36" t="s">
+        <v>315</v>
+      </c>
+      <c r="B29" s="36"/>
+      <c r="C29" s="36"/>
+    </row>
+    <row r="30" spans="1:3" ht="51.75" x14ac:dyDescent="0.2">
+      <c r="A30" s="37" t="s">
+        <v>316</v>
+      </c>
+      <c r="B30" s="37" t="s">
+        <v>317</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>318</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A29:C29"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>

</xml_diff>